<commit_message>
Fixed header/footer warning by removing header/footers from XY.xlsx input file, more code cleanup and bare-bones plot working
</commit_message>
<xml_diff>
--- a/Dotplots_update/14724_XY.xlsx
+++ b/Dotplots_update/14724_XY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\GitHub\personal-workspace\Dotplots_update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3EBE39-3985-4CFA-95DC-9229D7D8A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A465CE-DDA4-4100-9623-7A75EC2BE06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46650" yWindow="2760" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -262,12 +262,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2608,10 +2602,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;A</oddHeader>
-    <oddFooter>Page &amp;P</oddFooter>
-  </headerFooter>
+  <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>